<commit_message>
vault backup: 2025-02-13 09:26:53
</commit_message>
<xml_diff>
--- a/Timeplan.xlsx
+++ b/Timeplan.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mokslas\Thesis\obsidian\Thesis\Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FF3C70-83E8-4CAB-842D-DD835F325B37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5076C785-2DA8-4B32-8203-F5C61CECE844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="70">
   <si>
     <t>Week 1</t>
   </si>
@@ -365,12 +366,69 @@
       <t xml:space="preserve"> – additional time to account for mistakes, errors or hold-ups. Preparation for defense.</t>
     </r>
   </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Tue</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Thu</t>
+  </si>
+  <si>
+    <t>Fri</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Penguins Manuscript</t>
+  </si>
+  <si>
+    <r>
+      <t>Literature Analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Contact David regarding thesis defense deadlines.</t>
+  </si>
+  <si>
+    <r>
+      <t>Data Processing</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Liberation Sans"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Biweekly meeting with Torbern at 10:30 on Zoom</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,8 +483,42 @@
       <name val="Book Antiqua"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="Liberation Sans"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,18 +598,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FFD4EA6B"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -540,19 +644,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -586,35 +699,75 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="5" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
@@ -896,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="A1:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -914,36 +1067,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="20" t="s">
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="14">
+      <c r="A2" s="17">
         <v>45691</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="17">
         <v>45695</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -951,94 +1104,94 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="15">
+      <c r="A3" s="19">
         <v>45698</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="19">
         <v>45702</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="15">
+      <c r="A4" s="13">
         <v>45705</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="13">
         <v>45709</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="15">
+      <c r="A5" s="13">
         <v>45712</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B5" s="13">
         <v>45716</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="17"/>
+      <c r="F5" s="14"/>
       <c r="H5" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="15">
+      <c r="A6" s="13">
         <v>45719</v>
       </c>
-      <c r="B6" s="16">
+      <c r="B6" s="13">
         <v>45723</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="15">
+      <c r="A7" s="13">
         <v>45726</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="13">
         <v>45730</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1046,36 +1199,36 @@
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="15">
+      <c r="A8" s="13">
         <v>45733</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="13">
         <v>45737</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="15">
+      <c r="A9" s="13">
         <v>45740</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="13">
         <v>45744</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="7" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1083,36 +1236,36 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="15">
+      <c r="A10" s="13">
         <v>45747</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="13">
         <v>45751</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="15">
+      <c r="A11" s="13">
         <v>45754</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="13">
         <v>45758</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>24</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1120,299 +1273,296 @@
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="15">
+      <c r="A12" s="13">
         <v>45761</v>
       </c>
-      <c r="B12" s="16">
+      <c r="B12" s="13">
         <v>45765</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="15">
+      <c r="A13" s="13">
         <v>45768</v>
       </c>
-      <c r="B13" s="16">
+      <c r="B13" s="13">
         <v>45772</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="19" t="s">
+      <c r="H13" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="15">
+      <c r="A14" s="13">
         <v>45775</v>
       </c>
-      <c r="B14" s="16">
+      <c r="B14" s="13">
         <v>45779</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="19"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="15">
+      <c r="A15" s="13">
         <v>45782</v>
       </c>
-      <c r="B15" s="16">
+      <c r="B15" s="13">
         <v>45786</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="19" t="s">
+      <c r="H15" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="15">
+      <c r="A16" s="13">
         <v>45789</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="13">
         <v>45793</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>26</v>
       </c>
       <c r="G16" s="1"/>
-      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="15">
+      <c r="A17" s="13">
         <v>45796</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="13">
         <v>45800</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>27</v>
       </c>
       <c r="G17" s="1"/>
-      <c r="H17" s="19" t="s">
+      <c r="H17" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="15">
+      <c r="A18" s="13">
         <v>45803</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="13">
         <v>45807</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>35</v>
       </c>
       <c r="G18" s="1"/>
-      <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="15">
+      <c r="A19" s="13">
         <v>45810</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="13">
         <v>45814</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="15">
+      <c r="A20" s="13">
         <v>45817</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="13">
         <v>45821</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="11" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="15">
+      <c r="A21" s="13">
         <v>45824</v>
       </c>
-      <c r="B21" s="16">
+      <c r="B21" s="13">
         <v>45828</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="H21" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="16.5">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
-      <c r="H25" s="22"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
     </row>
     <row r="26" spans="1:8" ht="16.5">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="22"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
     </row>
     <row r="27" spans="1:8" ht="16.5">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="22"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
     </row>
     <row r="28" spans="1:8" ht="16.5">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:8" ht="16.5">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="22"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
     </row>
     <row r="30" spans="1:8" ht="16.5">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="22"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
+      <c r="H30" s="32"/>
     </row>
     <row r="31" spans="1:8" ht="16.5">
-      <c r="A31" s="22" t="s">
+      <c r="A31" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="22"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
     </row>
     <row r="32" spans="1:8" ht="16.5">
-      <c r="A32" s="22" t="s">
+      <c r="A32" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
     </row>
     <row r="33" spans="1:8" ht="16.5">
-      <c r="A33" s="22" t="s">
+      <c r="A33" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1430,4 +1580,704 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DB59D3C-F9B1-4979-8FEF-102FBBCACD92}">
+  <dimension ref="A1:X26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25.85546875" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="4" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="22.28515625" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" customWidth="1"/>
+    <col min="27" max="27" width="15.7109375" customWidth="1"/>
+    <col min="30" max="30" width="8.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17">
+        <v>45691</v>
+      </c>
+      <c r="C2" s="17">
+        <v>45695</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="P2" s="1"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="19">
+        <v>45698</v>
+      </c>
+      <c r="C3" s="19">
+        <v>45702</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13">
+        <v>45705</v>
+      </c>
+      <c r="C4" s="13">
+        <v>45709</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="P4" s="1"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13">
+        <v>45712</v>
+      </c>
+      <c r="C5" s="13">
+        <v>45716</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="13">
+        <v>45719</v>
+      </c>
+      <c r="C6" s="13">
+        <v>45723</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13">
+        <v>45726</v>
+      </c>
+      <c r="C7" s="13">
+        <v>45730</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="1"/>
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="13">
+        <v>45733</v>
+      </c>
+      <c r="C8" s="13">
+        <v>45737</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="1"/>
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13">
+        <v>45740</v>
+      </c>
+      <c r="C9" s="13">
+        <v>45744</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="1"/>
+      <c r="P9" s="1"/>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="13">
+        <v>45747</v>
+      </c>
+      <c r="C10" s="13">
+        <v>45751</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="1"/>
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13">
+        <v>45754</v>
+      </c>
+      <c r="C11" s="13">
+        <v>45758</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="1"/>
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13">
+        <v>45761</v>
+      </c>
+      <c r="C12" s="13">
+        <v>45765</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="1"/>
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>45768</v>
+      </c>
+      <c r="C13" s="13">
+        <v>45772</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13">
+        <v>45775</v>
+      </c>
+      <c r="C14" s="13">
+        <v>45779</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="13">
+        <v>45782</v>
+      </c>
+      <c r="C15" s="13">
+        <v>45786</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="13">
+        <v>45789</v>
+      </c>
+      <c r="C16" s="13">
+        <v>45793</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="13">
+        <v>45796</v>
+      </c>
+      <c r="C17" s="13">
+        <v>45800</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H17" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="13">
+        <v>45803</v>
+      </c>
+      <c r="C18" s="13">
+        <v>45807</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="L18" s="14"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="13">
+        <v>45810</v>
+      </c>
+      <c r="C19" s="13">
+        <v>45814</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="L19" s="14"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="13">
+        <v>45817</v>
+      </c>
+      <c r="C20" s="13">
+        <v>45821</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L20" s="14"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="13">
+        <v>45824</v>
+      </c>
+      <c r="C21" s="13">
+        <v>45828</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="L21" s="14"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="H22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>